<commit_message>
added new beginning conditions for special cases
</commit_message>
<xml_diff>
--- a/DIRAC_MATLAB/files/Data.xlsx
+++ b/DIRAC_MATLAB/files/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\MATLAB\Dirac\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\Shooting_Dirac\DIRAC_MATLAB\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0C9FFEF-DB2E-4E89-984B-4DD227E1F23E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F229ACDB-1852-424D-B3D2-1BF17BA4A391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -599,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L90"/>
+  <dimension ref="A1:N90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="N85" sqref="N85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3651,7 +3651,7 @@
         <v>75325975485.050598</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
@@ -3689,7 +3689,7 @@
         <v>525360.16329619673</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>-99192.520966574462</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>37789384761.680717</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
@@ -3803,7 +3803,7 @@
         <v>-557.95757720783695</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
@@ -3841,7 +3841,7 @@
         <v>46.80214225709603</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>1024593535.344329</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
       </c>
@@ -3914,10 +3914,13 @@
         <v>0.03</v>
       </c>
       <c r="L87">
+        <v>1</v>
+      </c>
+      <c r="N87">
         <v>-419612941.28389442</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>86</v>
       </c>
@@ -3955,7 +3958,7 @@
         <v>157573686221773.5</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
@@ -3993,7 +3996,7 @@
         <v>-12058514.909206441</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
fixed data with initial conds
</commit_message>
<xml_diff>
--- a/DIRAC_MATLAB/files/Data.xlsx
+++ b/DIRAC_MATLAB/files/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\Shooting_Dirac\DIRAC_MATLAB\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F229ACDB-1852-424D-B3D2-1BF17BA4A391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA7EDC09-B914-4155-A0DF-164AE47B8011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="73">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -85,27 +85,6 @@
     <t>40Ca 1f5/2</t>
   </si>
   <si>
-    <t>48Ca 1d5/2</t>
-  </si>
-  <si>
-    <t>48Ca 2s1/2</t>
-  </si>
-  <si>
-    <t>48Ca 1d3/2</t>
-  </si>
-  <si>
-    <t>48Ca 1f7/2</t>
-  </si>
-  <si>
-    <t>48Ca 2p3/2</t>
-  </si>
-  <si>
-    <t>48Ca 2p1/2</t>
-  </si>
-  <si>
-    <t>48Ca 1f5/2</t>
-  </si>
-  <si>
     <t>56Ni 1f7/2</t>
   </si>
   <si>
@@ -139,33 +118,6 @@
     <t>100Sn 2d3/2</t>
   </si>
   <si>
-    <t>132Sn 1g7/2</t>
-  </si>
-  <si>
-    <t>132Sn 2d5/2</t>
-  </si>
-  <si>
-    <t>132Sn 3s1/2</t>
-  </si>
-  <si>
-    <t>132Sn 1h11/2</t>
-  </si>
-  <si>
-    <t>132Sn 2d3/2</t>
-  </si>
-  <si>
-    <t>132Sn 2f7/2</t>
-  </si>
-  <si>
-    <t>132Sn 3p3/2</t>
-  </si>
-  <si>
-    <t>132Sn 1h9/2</t>
-  </si>
-  <si>
-    <t>132Sn 2f5/2</t>
-  </si>
-  <si>
     <t>208Pb 1h9/2</t>
   </si>
   <si>
@@ -211,12 +163,6 @@
     <t>100Sn 2p3/2</t>
   </si>
   <si>
-    <t>132Sn 2p1/2</t>
-  </si>
-  <si>
-    <t>132Sn 1g9/2</t>
-  </si>
-  <si>
     <t>208Pb 1g7/2</t>
   </si>
   <si>
@@ -236,6 +182,63 @@
   </si>
   <si>
     <t>a0_d</t>
+  </si>
+  <si>
+    <t>B_init</t>
+  </si>
+  <si>
+    <t>132Cs 1g7/2</t>
+  </si>
+  <si>
+    <t>132Cs 2d5/2</t>
+  </si>
+  <si>
+    <t>132Cs 3s1/2</t>
+  </si>
+  <si>
+    <t>132Cs 1h11/2</t>
+  </si>
+  <si>
+    <t>132Cs 2d3/2</t>
+  </si>
+  <si>
+    <t>132Cs 2f7/2</t>
+  </si>
+  <si>
+    <t>132Cs 3p3/2</t>
+  </si>
+  <si>
+    <t>132Cs 1h9/2</t>
+  </si>
+  <si>
+    <t>132Cs 2f5/2</t>
+  </si>
+  <si>
+    <t>132Cs 2p1/2</t>
+  </si>
+  <si>
+    <t>132Cs 1g9/2</t>
+  </si>
+  <si>
+    <t>48Cd 1d5/2</t>
+  </si>
+  <si>
+    <t>48Cd 2s1/2</t>
+  </si>
+  <si>
+    <t>48Cd 1d3/2</t>
+  </si>
+  <si>
+    <t>48Cd 1f7/2</t>
+  </si>
+  <si>
+    <t>48Cd 2p3/2</t>
+  </si>
+  <si>
+    <t>48Cd 2p1/2</t>
+  </si>
+  <si>
+    <t>48Cd 1f5/2</t>
   </si>
 </sst>
 </file>
@@ -292,11 +295,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,19 +603,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N90"/>
+  <dimension ref="A1:M90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="N85" sqref="N85"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="N80" sqref="N80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -646,10 +652,13 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -686,8 +695,11 @@
       <c r="L2">
         <v>1.658997792719755</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <v>-15.66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -724,8 +736,11 @@
       <c r="L3">
         <v>9016258.8276325949</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <v>-4.1399999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -762,8 +777,11 @@
       <c r="L4">
         <v>-22.10063499911136</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>-3.27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -800,8 +818,11 @@
       <c r="L5">
         <v>314608.70648511662</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>-22.39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -838,8 +859,11 @@
       <c r="L6">
         <v>-2.2286498625439428</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>-18.190000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -876,8 +900,11 @@
       <c r="L7">
         <v>297.73550585535861</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>-15.64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -914,8 +941,11 @@
       <c r="L8">
         <v>9257096.9378283992</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>-8.36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -952,8 +982,11 @@
       <c r="L9">
         <v>-51457.723733753708</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>-5.84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -990,8 +1023,11 @@
       <c r="L10">
         <v>-6.3049884373868244</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>-4.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1028,13 +1064,16 @@
       <c r="L11">
         <v>3498207.161153608</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>-1.56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="C12">
         <v>-1</v>
@@ -1066,13 +1105,16 @@
       <c r="L12">
         <v>253213.2389241411</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>-15.61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="C13">
         <v>-1</v>
@@ -1104,13 +1146,16 @@
       <c r="L13">
         <v>-2.4715668618765729</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>-12.55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="C14">
         <v>-1</v>
@@ -1142,13 +1187,16 @@
       <c r="L14">
         <v>70.762330378772134</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <v>-12.53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="C15">
         <v>-1</v>
@@ -1180,13 +1228,16 @@
       <c r="L15">
         <v>350157548.95774019</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="C16">
         <v>-1</v>
@@ -1218,13 +1269,16 @@
       <c r="L16">
         <v>-1613.245464568254</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>-4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="C17">
         <v>-1</v>
@@ -1256,13 +1310,16 @@
       <c r="L17">
         <v>-11.04207631205419</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>-2.86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="C18">
         <v>-1</v>
@@ -1294,13 +1351,16 @@
       <c r="L18">
         <v>174399.86011193239</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C19">
         <v>-1</v>
@@ -1332,13 +1392,16 @@
       <c r="L19">
         <v>1359019.802977222</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>-16.64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C20">
         <v>-1</v>
@@ -1370,13 +1433,16 @@
       <c r="L20">
         <v>-1534.599312857227</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <v>-10.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C21">
         <v>-1</v>
@@ -1408,13 +1474,16 @@
       <c r="L21">
         <v>12958.776093654729</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>-9.48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C22">
         <v>-1</v>
@@ -1446,13 +1515,16 @@
       <c r="L22">
         <v>-1.3835744761114881</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <v>-9.1300000000000008</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C23">
         <v>-1</v>
@@ -1484,13 +1556,16 @@
       <c r="L23">
         <v>-0.1071824492262787</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23">
+        <v>-18.38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C24">
         <v>-1</v>
@@ -1522,13 +1597,16 @@
       <c r="L24">
         <v>4041967.2274771328</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M24">
+        <v>-17.93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C25">
         <v>-1</v>
@@ -1560,13 +1638,16 @@
       <c r="L25">
         <v>-15784.53832047469</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25">
+        <v>-11.13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C26">
         <v>-1</v>
@@ -1598,13 +1679,16 @@
       <c r="L26">
         <v>446520.43705178762</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26">
+        <v>-10.93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C27">
         <v>-1</v>
@@ -1636,13 +1720,16 @@
       <c r="L27">
         <v>3.0801305584999938</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M27">
+        <v>-9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C28">
         <v>-1</v>
@@ -1674,13 +1761,16 @@
       <c r="L28">
         <v>16775876805.373249</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M28">
+        <v>-8.6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C29">
         <v>-1</v>
@@ -1712,13 +1802,16 @@
       <c r="L29">
         <v>-112.0143097572699</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M29">
+        <v>-9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="C30">
         <v>-1</v>
@@ -1750,13 +1843,16 @@
       <c r="L30">
         <v>147182.2165906617</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M30">
+        <v>-9.75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="C31">
         <v>-1</v>
@@ -1788,13 +1884,16 @@
       <c r="L31">
         <v>-19649.642170071718</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M31">
+        <v>-8.9700000000000006</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C32">
         <v>-1</v>
@@ -1826,13 +1925,16 @@
       <c r="L32">
         <v>-0.1257702587890297</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M32">
+        <v>-7.64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="C33">
         <v>-1</v>
@@ -1864,13 +1966,16 @@
       <c r="L33">
         <v>8128748557.6012135</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M33">
+        <v>-7.54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="C34">
         <v>-1</v>
@@ -1902,13 +2007,16 @@
       <c r="L34">
         <v>-244.0804419055365</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M34">
+        <v>-7.31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="C35">
         <v>-1</v>
@@ -1940,13 +2048,16 @@
       <c r="L35">
         <v>55806.869863989872</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M35">
+        <v>-2.4700000000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C36">
         <v>-1</v>
@@ -1972,19 +2083,22 @@
       <c r="J36">
         <v>0.15</v>
       </c>
-      <c r="K36">
-        <v>0.03</v>
+      <c r="K36" s="2">
+        <v>5.6402416846005603E-2</v>
       </c>
       <c r="L36">
         <v>-35.950913858880362</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M36" s="2">
+        <v>3.07944307104533</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="C37">
         <v>-1</v>
@@ -2016,13 +2130,16 @@
       <c r="L37">
         <v>30363070027.814919</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M37">
+        <v>-0.86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="C38">
         <v>-1</v>
@@ -2048,19 +2165,22 @@
       <c r="J38">
         <v>0.15</v>
       </c>
-      <c r="K38">
-        <v>0.03</v>
+      <c r="K38" s="2">
+        <v>1.1599837858531701E-2</v>
       </c>
       <c r="L38">
         <v>574.95849566698212</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M38" s="2">
+        <v>1.7067888766485799</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C39">
         <v>-1</v>
@@ -2092,13 +2212,16 @@
       <c r="L39">
         <v>1270266.4230192541</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M39">
+        <v>-11.4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C40">
         <v>-1</v>
@@ -2130,13 +2253,16 @@
       <c r="L40">
         <v>-621877.24272524554</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M40">
+        <v>-9.81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="C41">
         <v>-1</v>
@@ -2168,13 +2294,16 @@
       <c r="L41">
         <v>546338971647.59167</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M41">
+        <v>-9.24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="C42">
         <v>-1</v>
@@ -2206,13 +2335,16 @@
       <c r="L42">
         <v>1750.9217689392101</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M42">
+        <v>-8.26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C43">
         <v>-1</v>
@@ -2244,13 +2376,16 @@
       <c r="L43">
         <v>36.016079531073188</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M43">
+        <v>-7.94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C44">
         <v>-1</v>
@@ -2276,19 +2411,22 @@
       <c r="J44">
         <v>0.15</v>
       </c>
-      <c r="K44">
-        <v>0.03</v>
+      <c r="K44" s="2">
+        <v>0.14978896672456199</v>
       </c>
       <c r="L44">
         <v>-1.2634501209437359E-2</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M44" s="2">
+        <v>-6.3046625379287899</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="C45">
         <v>-1</v>
@@ -2320,13 +2458,16 @@
       <c r="L45">
         <v>-310950830.4587937</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M45">
+        <v>-3.94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="C46">
         <v>-1</v>
@@ -2358,13 +2499,16 @@
       <c r="L46">
         <v>47775089907.640579</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M46">
+        <v>-3.16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C47">
         <v>-1</v>
@@ -2396,13 +2540,16 @@
       <c r="L47">
         <v>9086320298821846</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M47">
+        <v>-2.5099999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C48">
         <v>-1</v>
@@ -2428,19 +2575,22 @@
       <c r="J48">
         <v>0.15</v>
       </c>
-      <c r="K48">
-        <v>0.03</v>
+      <c r="K48" s="2">
+        <v>4.0215322760543501E-2</v>
       </c>
       <c r="L48">
         <v>-1017.275231126728</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M48" s="2">
+        <v>1.4712843833253799</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C49">
         <v>-1</v>
@@ -2466,19 +2616,22 @@
       <c r="J49">
         <v>0.17</v>
       </c>
-      <c r="K49">
-        <v>0.03</v>
+      <c r="K49" s="2">
+        <v>1.3531587729214201E-2</v>
       </c>
       <c r="L49">
         <v>0.36357048751758331</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M49" s="2">
+        <v>2.4716196788386999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="C50">
         <v>-1</v>
@@ -2504,14 +2657,17 @@
       <c r="J50">
         <v>0.15</v>
       </c>
-      <c r="K50">
-        <v>0.03</v>
+      <c r="K50" s="2">
+        <v>1.48771405461984E-2</v>
       </c>
       <c r="L50">
         <v>2265171.199967925</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M50" s="2">
+        <v>-0.445616823906819</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2548,8 +2704,11 @@
       <c r="L51">
         <v>3.9451447635704802</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M51">
+        <v>-12.13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -2586,8 +2745,11 @@
       <c r="L52">
         <v>1752416.074061088</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M52">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -2624,13 +2786,16 @@
       <c r="L53">
         <v>-211.5490335700801</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M53">
+        <v>-0.11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -2662,8 +2827,11 @@
       <c r="L54">
         <v>-8604.1055998090505</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M54">
+        <v>4.6879999999999997</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -2700,8 +2868,11 @@
       <c r="L55">
         <v>1553689.5594360619</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M55">
+        <v>-15.07</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -2738,8 +2909,11 @@
       <c r="L56">
         <v>-23.820771819745229</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M56">
+        <v>-10.92</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -2776,8 +2950,11 @@
       <c r="L57">
         <v>2255.2395656699341</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M57">
+        <v>-8.33</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -2814,8 +2991,11 @@
       <c r="L58">
         <v>288190413.42597312</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M58">
+        <v>-1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -2852,13 +3032,16 @@
       <c r="L59">
         <v>-68732.544020347385</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M59">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -2890,13 +3073,16 @@
       <c r="L60">
         <v>14700.510065461</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M60">
+        <v>-21.47</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -2928,13 +3114,16 @@
       <c r="L61">
         <v>81.290921199096033</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M61">
+        <v>-16.18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -2966,13 +3155,16 @@
       <c r="L62">
         <v>-3.3310855333966991</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M62">
+        <v>-16.100000000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -3004,13 +3196,16 @@
       <c r="L63">
         <v>9409642.5446125884</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M63">
+        <v>-9.35</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -3042,13 +3237,16 @@
       <c r="L64">
         <v>-19683.971481754339</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M64">
+        <v>-6.44</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -3080,13 +3278,16 @@
       <c r="L65">
         <v>-22.189061181308549</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M65">
+        <v>-4.6399999999999997</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -3118,13 +3319,16 @@
       <c r="L66">
         <v>39541010.472970963</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M66">
+        <v>-7.17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -3156,13 +3360,16 @@
       <c r="L67">
         <v>-136437.80210508959</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M67">
+        <v>-0.69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -3194,13 +3401,16 @@
       <c r="L68">
         <v>-23299.221247090682</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M68">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -3232,13 +3442,16 @@
       <c r="L69">
         <v>-76204.656391052646</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M69">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -3270,13 +3483,16 @@
       <c r="L70">
         <v>93068.928539224566</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M70">
+        <v>-8.7100000000000009</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -3308,13 +3524,16 @@
       <c r="L71">
         <v>-40768.689808628929</v>
       </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M71">
+        <v>-6.38</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -3346,13 +3565,16 @@
       <c r="L72">
         <v>-66.04785857237276</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M72">
+        <v>-3.53</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -3384,13 +3606,16 @@
       <c r="L73">
         <v>13583849071.904091</v>
       </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M73">
+        <v>-2.92</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -3416,19 +3641,22 @@
       <c r="J74">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="K74">
-        <v>0.03</v>
+      <c r="K74" s="2">
+        <v>7.7358330060925597E-3</v>
       </c>
       <c r="L74">
         <v>-575325.02182732651</v>
       </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M74" s="2">
+        <v>2.2031135908367001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -3460,13 +3688,16 @@
       <c r="L75">
         <v>-0.2483417188349433</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M75">
+        <v>-16.010000000000002</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -3498,13 +3729,16 @@
       <c r="L76">
         <v>61004761.681937017</v>
       </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M76">
+        <v>-15.71</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -3536,13 +3770,16 @@
       <c r="L77">
         <v>695529.6132045557</v>
       </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M77">
+        <v>-9.68</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -3574,13 +3811,16 @@
       <c r="L78">
         <v>-61771.2895248696</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M78">
+        <v>-8.7200000000000006</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="C79">
         <v>1</v>
@@ -3606,19 +3846,22 @@
       <c r="J79">
         <v>0.1</v>
       </c>
-      <c r="K79">
-        <v>0.03</v>
+      <c r="K79" s="2">
+        <v>5.8415698900729202E-2</v>
       </c>
       <c r="L79">
         <v>-363.25484034743658</v>
       </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M79" s="2">
+        <v>-3.3377705686825201</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -3650,13 +3893,16 @@
       <c r="L80">
         <v>75325975485.050598</v>
       </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M80">
+        <v>-6.89</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -3688,13 +3934,16 @@
       <c r="L81">
         <v>525360.16329619673</v>
       </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M81">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -3726,13 +3975,16 @@
       <c r="L82">
         <v>-99192.520966574462</v>
       </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M82">
+        <v>-9.82</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -3764,13 +4016,16 @@
       <c r="L83">
         <v>37789384761.680717</v>
       </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M83">
+        <v>-9.36</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="C84">
         <v>1</v>
@@ -3796,19 +4051,22 @@
       <c r="J84">
         <v>0.15</v>
       </c>
-      <c r="K84">
-        <v>0.03</v>
+      <c r="K84" s="2">
+        <v>4.1984151677682997E-2</v>
       </c>
       <c r="L84">
         <v>-557.95757720783695</v>
       </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M84" s="2">
+        <v>-0.60643633449573298</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="C85">
         <v>1</v>
@@ -3834,19 +4092,22 @@
       <c r="J85">
         <v>0.15</v>
       </c>
-      <c r="K85">
-        <v>0.03</v>
+      <c r="K85" s="2">
+        <v>4.2525509164617101E-2</v>
       </c>
       <c r="L85">
         <v>46.80214225709603</v>
       </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M85" s="2">
+        <v>-0.82302655006273895</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C86">
         <v>1</v>
@@ -3878,13 +4139,16 @@
       <c r="L86">
         <v>1024593535.344329</v>
       </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M86">
+        <v>-3.8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C87">
         <v>1</v>
@@ -3910,22 +4174,22 @@
       <c r="J87">
         <v>0.15</v>
       </c>
-      <c r="K87">
-        <v>0.03</v>
+      <c r="K87" s="2">
+        <v>1.8612477096098399E-2</v>
       </c>
       <c r="L87">
-        <v>1</v>
-      </c>
-      <c r="N87">
         <v>-419612941.28389442</v>
       </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M87" s="2">
+        <v>-0.78804620529660396</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="C88">
         <v>1</v>
@@ -3957,13 +4221,16 @@
       <c r="L88">
         <v>157573686221773.5</v>
       </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M88">
+        <v>-2.1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="C89">
         <v>1</v>
@@ -3989,19 +4256,22 @@
       <c r="J89">
         <v>0.15</v>
       </c>
-      <c r="K89">
-        <v>0.03</v>
+      <c r="K89" s="2">
+        <v>4.1478457371563103E-2</v>
       </c>
       <c r="L89">
         <v>-12058514.909206441</v>
       </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M89" s="2">
+        <v>2.05124484053625</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="C90">
         <v>1</v>
@@ -4027,11 +4297,14 @@
       <c r="J90">
         <v>0.15</v>
       </c>
-      <c r="K90">
-        <v>0.03</v>
+      <c r="K90" s="2">
+        <v>4.67763884005684E-2</v>
       </c>
       <c r="L90">
         <v>6657046.3848697105</v>
+      </c>
+      <c r="M90" s="2">
+        <v>2.51801186433608</v>
       </c>
     </row>
   </sheetData>

</xml_diff>